<commit_message>
Run much more securely
A couple of fixes:

1. Avoid timeouts when calling GHCI -- there is nothing we can do apart from block, really.
2. Avoid multithreaded calls into GHCI -- these make no sense anyway.
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcus\Projects\Haxcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C9F054-F81F-4E0A-8152-CD24D85D9637}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A0F614-81A3-44D8-B6E0-DDA5041A8E45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2310" yWindow="570" windowWidth="16760" windowHeight="8940" xr2:uid="{B5F9E055-31D7-434A-8084-17B12F6C2AA8}"/>
   </bookViews>
@@ -374,7 +374,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Add hxLoad and hxReload
Functions to load and reload Haskell modules
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcus\Projects\Haxcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A0F614-81A3-44D8-B6E0-DDA5041A8E45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587A46FA-4ED7-446A-980C-1BA45A67220C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2310" yWindow="570" windowWidth="16760" windowHeight="8940" xr2:uid="{B5F9E055-31D7-434A-8084-17B12F6C2AA8}"/>
   </bookViews>
@@ -374,7 +374,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -412,7 +412,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
-        <f ca="1">_xll.hxRaw(":l C:\Users\marcus\Projects\Haxcel\test.hs")</f>
+        <f ca="1">_xll.hxLoad("C:\Users\marcus\Projects\Haxcel\test.hs")</f>
         <v>[1 of 1] Compiling Main             ( C:\Users\marcus\Projects\Haxcel\test.hs, interpreted )_x000D_
 Ok, one module loaded._x000D_</v>
       </c>

</xml_diff>